<commit_message>
Update project, fix README, HOWUSE
</commit_message>
<xml_diff>
--- a/Planilha de Críticas.xlsx
+++ b/Planilha de Críticas.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eliasp\Documents\GitHub\python-automatics-data-alterations-in-xml-file\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elias\Documents\GitHub\python-automatics-data-alterations-in-xml-file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75E1023F-5C25-4C6C-A41E-5711618F057D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4583B294-4B3F-454F-8A3F-3C892AD5E609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="0" windowWidth="15405" windowHeight="10920" xr2:uid="{2CB27820-A556-4FB3-A9D8-7569D697D985}"/>
+    <workbookView xWindow="4515" yWindow="2325" windowWidth="16200" windowHeight="9360" activeTab="1" xr2:uid="{2CB27820-A556-4FB3-A9D8-7569D697D985}"/>
   </bookViews>
   <sheets>
-    <sheet name="1" sheetId="2" r:id="rId1"/>
-    <sheet name="2" sheetId="3" r:id="rId2"/>
+    <sheet name="Dados" sheetId="2" r:id="rId1"/>
+    <sheet name="Valores" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Número da conta</t>
   </si>
@@ -81,49 +81,19 @@
     <t>Código de despesa (novo)</t>
   </si>
   <si>
-    <t>1200288832</t>
-  </si>
-  <si>
-    <t>1200108505</t>
-  </si>
-  <si>
-    <t>98020315</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>00</t>
-  </si>
-  <si>
-    <t>79419356</t>
-  </si>
-  <si>
-    <t>1200329452</t>
+    <t>70223777</t>
   </si>
   <si>
     <t>19</t>
   </si>
   <si>
-    <t>90289870</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>01</t>
-  </si>
-  <si>
-    <t>90022181</t>
-  </si>
-  <si>
-    <t>04</t>
-  </si>
-  <si>
-    <t>40202615</t>
-  </si>
-  <si>
-    <t>11</t>
+    <t>50</t>
+  </si>
+  <si>
+    <t>62,59</t>
+  </si>
+  <si>
+    <t>70</t>
   </si>
 </sst>
 </file>
@@ -165,13 +135,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -181,68 +148,68 @@
   <dxfs count="19">
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -261,33 +228,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CBA62B90-882A-4BF9-8830-CAF827AD06C4}" name="Tabela132" displayName="Tabela132" ref="A1:K11" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" headerRowCellStyle="Normal" dataCellStyle="Normal">
-  <autoFilter ref="A1:K11" xr:uid="{CBA62B90-882A-4BF9-8830-CAF827AD06C4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CBA62B90-882A-4BF9-8830-CAF827AD06C4}" name="Tabela132" displayName="Tabela132" ref="A1:K2" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" headerRowCellStyle="Normal" dataCellStyle="Normal">
+  <autoFilter ref="A1:K2" xr:uid="{CBA62B90-882A-4BF9-8830-CAF827AD06C4}"/>
   <tableColumns count="11">
-    <tableColumn id="13" xr3:uid="{06C614F5-975F-4B1A-9F7C-1B1B223F90E9}" name="Número da conta" dataDxfId="10" dataCellStyle="Normal"/>
-    <tableColumn id="1" xr3:uid="{C621B725-797C-4D67-9A0F-E59B73B613A3}" name="Código do procedimento (atual)" dataDxfId="9" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{C41B8A8A-18B2-451B-A1F0-0AA53AABFCE2}" name="Código do procedimento (novo)" dataDxfId="8" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{6B6C2E86-61A2-46B0-9A14-ED8E829E9EBF}" name="Tipo de tabela (atual)" dataDxfId="7" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{2538689F-463F-48B1-A151-46DC98BD40E4}" name="Tipo de tabela (novo)" dataDxfId="6" dataCellStyle="Normal"/>
-    <tableColumn id="6" xr3:uid="{FE55CA78-5D09-4FEB-A98C-731905E074A1}" name="Grau de participação (atual)" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{F3B0A441-345D-4A45-9615-25EE4E899A96}" name="Grau de participação (novo)" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{488192F4-8EB7-4ACA-AC25-AE49E4E77594}" name="Código de despesa (atual)" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{922EC5F7-10DB-4286-8B43-1B64D0F9B443}" name="Código de despesa (novo)" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{2D918A51-1747-439F-B24F-0EF57A6B36AD}" name="Unidade de medida (atual)" dataDxfId="1" dataCellStyle="Normal"/>
-    <tableColumn id="12" xr3:uid="{BEA4C293-0DC8-4FF8-9304-A42886CDFA65}" name="Unidade de medida (novo)" dataDxfId="0" dataCellStyle="Normal"/>
+    <tableColumn id="13" xr3:uid="{06C614F5-975F-4B1A-9F7C-1B1B223F90E9}" name="Número da conta" dataDxfId="16" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{C621B725-797C-4D67-9A0F-E59B73B613A3}" name="Código do procedimento (atual)" dataDxfId="1" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{C41B8A8A-18B2-451B-A1F0-0AA53AABFCE2}" name="Código do procedimento (novo)" dataDxfId="15" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{6B6C2E86-61A2-46B0-9A14-ED8E829E9EBF}" name="Tipo de tabela (atual)" dataDxfId="2" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{2538689F-463F-48B1-A151-46DC98BD40E4}" name="Tipo de tabela (novo)" dataDxfId="14" dataCellStyle="Normal"/>
+    <tableColumn id="6" xr3:uid="{FE55CA78-5D09-4FEB-A98C-731905E074A1}" name="Grau de participação (atual)" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{F3B0A441-345D-4A45-9615-25EE4E899A96}" name="Grau de participação (novo)" dataDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{488192F4-8EB7-4ACA-AC25-AE49E4E77594}" name="Código de despesa (atual)" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{922EC5F7-10DB-4286-8B43-1B64D0F9B443}" name="Código de despesa (novo)" dataDxfId="10"/>
+    <tableColumn id="11" xr3:uid="{2D918A51-1747-439F-B24F-0EF57A6B36AD}" name="Unidade de medida (atual)" dataDxfId="9" dataCellStyle="Normal"/>
+    <tableColumn id="12" xr3:uid="{BEA4C293-0DC8-4FF8-9304-A42886CDFA65}" name="Unidade de medida (novo)" dataDxfId="8" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{EF3F8EE2-2535-4055-995F-58277DA69320}" name="Tabela3" displayName="Tabela3" ref="A1:D8" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
-  <autoFilter ref="A1:D8" xr:uid="{EF3F8EE2-2535-4055-995F-58277DA69320}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{EF3F8EE2-2535-4055-995F-58277DA69320}" name="Tabela3" displayName="Tabela3" ref="A1:D2" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:D2" xr:uid="{EF3F8EE2-2535-4055-995F-58277DA69320}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E041450B-B9A8-4984-80F1-F392EA1249E0}" name="Número da conta" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{34DF0F1F-4A50-4495-9A62-004334AB22FA}" name="Código do procedimento" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{AA7D6B72-0CFC-4D03-95C6-61EB48D14747}" name="Valor unitário (atual)" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{3D107E8F-238F-4D9E-A978-F4020F61C26E}" name="Valor unitário (novo)" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{E041450B-B9A8-4984-80F1-F392EA1249E0}" name="Número da conta" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{34DF0F1F-4A50-4495-9A62-004334AB22FA}" name="Código do procedimento" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{AA7D6B72-0CFC-4D03-95C6-61EB48D14747}" name="Valor unitário (atual)" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{3D107E8F-238F-4D9E-A978-F4020F61C26E}" name="Valor unitário (novo)" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -590,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C61B51D-8349-4064-B6F9-68B2ADB2D555}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,170 +610,23 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="E2" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -822,8 +642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{659A0C52-99B9-496E-B347-5D1AC694609B}">
   <dimension ref="A1:S17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -856,45 +676,15 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="S13" t="str">
@@ -928,7 +718,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>